<commit_message>
adding json for configuration
</commit_message>
<xml_diff>
--- a/test_data/orange_test_data.xlsx
+++ b/test_data/orange_test_data.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\hybrid_framework\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DCD01E6-167D-49C6-8810-5DE17DE51C0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D7969F5-2A5B-4DE7-985A-54919B66B26E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3195" yWindow="1725" windowWidth="21600" windowHeight="8220" xr2:uid="{7EB96F12-122D-4A74-A5EA-B63A96173B33}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{7EB96F12-122D-4A74-A5EA-B63A96173B33}"/>
   </bookViews>
   <sheets>
     <sheet name="test_add_valid_employee" sheetId="1" r:id="rId1"/>
+    <sheet name="test_invalid_upload_file" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="20">
   <si>
     <t>Username</t>
   </si>
@@ -84,6 +85,18 @@
   </si>
   <si>
     <t>Roj Anta</t>
+  </si>
+  <si>
+    <t>file_path</t>
+  </si>
+  <si>
+    <t>expected_error</t>
+  </si>
+  <si>
+    <t>File type not allowed</t>
+  </si>
+  <si>
+    <t>C:\output.txt</t>
   </si>
 </sst>
 </file>
@@ -119,8 +132,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -437,8 +453,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D829E8E7-3474-434C-B624-5E077F37144F}">
   <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -516,4 +532,52 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8812F050-A920-4A38-B435-847818E512F2}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="17.85546875" customWidth="1"/>
+    <col min="4" max="4" width="24.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>